<commit_message>
update new source in 11jan2018
</commit_message>
<xml_diff>
--- a/data/TC003.xlsx
+++ b/data/TC003.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Password</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>kannan.d@gmail.com</t>
+  </si>
+  <si>
+    <t>9638527410</t>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
 </sst>
 </file>
@@ -159,13 +165,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -471,7 +479,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,14 +543,14 @@
       <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2">
-        <v>9638527410</v>
+      <c r="H2" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="3">
-        <v>123456</v>
+      <c r="J2" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>